<commit_message>
Planned VS Actual Velocity
Upon completing the Sprint, we have calculated our actual velocity and estimated our planned velocity for the next Sprint.
</commit_message>
<xml_diff>
--- a/Sprint 1/Sprint_Backlog/Planned VS Actual Velocity.xlsx
+++ b/Sprint 1/Sprint_Backlog/Planned VS Actual Velocity.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikol\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikol\Documents\GitHub\AC31007-Coursework-Team-2\Sprint 1\Sprint_Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4864C04-412A-4E07-BE8C-5C1A727E7F84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBB4BF0-641E-4ACB-936F-53EDF032887A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8865F123-9DFE-4D00-84C2-5B85458E96D5}"/>
   </bookViews>
@@ -306,6 +306,9 @@
                 <c:pt idx="0">
                   <c:v>30</c:v>
                 </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -380,6 +383,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1532,7 +1538,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1557,13 +1563,17 @@
       <c r="B2" s="2">
         <v>30</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="2">
+        <v>40</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="3">
+        <v>35</v>
+      </c>
       <c r="C3" s="3"/>
     </row>
   </sheetData>

</xml_diff>